<commit_message>
/ ‘Microsoft Select plus agreement prices - India.xlsx’ - ‘~$Microsoft Select plus agreement prices - India.xlsx’
</commit_message>
<xml_diff>
--- a/Microsoft Select plus agreement prices - India.xlsx
+++ b/Microsoft Select plus agreement prices - India.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Micosoft Licenses Select Plus Agreement</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Windows server 2008 CAL Licenses</t>
+  </si>
+  <si>
+    <t>RAMESH</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -692,11 +695,11 @@
         <v>500</v>
       </c>
       <c r="J6" s="13">
-        <f>I6-G6</f>
+        <f t="shared" ref="J6:J12" si="0">I6-G6</f>
         <v>88.972222222222229</v>
       </c>
       <c r="K6" s="13">
-        <f>J6*F6</f>
+        <f t="shared" ref="K6:K12" si="1">J6*F6</f>
         <v>1245.6111111111113</v>
       </c>
     </row>
@@ -717,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="10">
-        <f t="shared" ref="F7:F12" si="0">SUM(C7:E7)</f>
+        <f t="shared" ref="F7:F12" si="2">SUM(C7:E7)</f>
         <v>2</v>
       </c>
       <c r="G7" s="12">
@@ -725,18 +728,18 @@
         <v>400.97222222222223</v>
       </c>
       <c r="H7" s="12">
-        <f t="shared" ref="H7:H12" si="1">G7*F7</f>
+        <f t="shared" ref="H7:H12" si="3">G7*F7</f>
         <v>801.94444444444446</v>
       </c>
       <c r="I7" s="12">
         <v>500</v>
       </c>
       <c r="J7" s="14">
-        <f>I7-G7</f>
+        <f t="shared" si="0"/>
         <v>99.027777777777771</v>
       </c>
       <c r="K7" s="14">
-        <f>J7*F7</f>
+        <f t="shared" si="1"/>
         <v>198.05555555555554</v>
       </c>
     </row>
@@ -757,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G8" s="12">
@@ -765,18 +768,18 @@
         <v>303.84722222222223</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2430.7777777777778</v>
       </c>
       <c r="I8" s="12">
         <v>350</v>
       </c>
       <c r="J8" s="14">
-        <f>I8-G8</f>
+        <f t="shared" si="0"/>
         <v>46.152777777777771</v>
       </c>
       <c r="K8" s="14">
-        <f>J8*F8</f>
+        <f t="shared" si="1"/>
         <v>369.22222222222217</v>
       </c>
     </row>
@@ -797,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="G9" s="12">
@@ -805,18 +808,18 @@
         <v>210.83333333333334</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13704.166666666668</v>
       </c>
       <c r="I9" s="12">
         <v>285</v>
       </c>
       <c r="J9" s="14">
-        <f>I9-G9</f>
+        <f t="shared" si="0"/>
         <v>74.166666666666657</v>
       </c>
       <c r="K9" s="14">
-        <f>J9*F9</f>
+        <f t="shared" si="1"/>
         <v>4820.833333333333</v>
       </c>
     </row>
@@ -837,7 +840,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G10" s="12">
@@ -845,18 +848,18 @@
         <v>210.81944444444446</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16865.555555555555</v>
       </c>
       <c r="I10" s="12">
         <v>140</v>
       </c>
       <c r="J10" s="14">
-        <f>I10-G10</f>
+        <f t="shared" si="0"/>
         <v>-70.819444444444457</v>
       </c>
       <c r="K10" s="14">
-        <f>J10*F10</f>
+        <f t="shared" si="1"/>
         <v>-5665.5555555555566</v>
       </c>
     </row>
@@ -877,7 +880,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="G11" s="12">
@@ -885,18 +888,18 @@
         <v>38.25</v>
       </c>
       <c r="H11" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7650</v>
       </c>
       <c r="I11" s="12">
         <v>51</v>
       </c>
       <c r="J11" s="14">
-        <f>I11-G11</f>
+        <f t="shared" si="0"/>
         <v>12.75</v>
       </c>
       <c r="K11" s="14">
-        <f>J11*F11</f>
+        <f t="shared" si="1"/>
         <v>2550</v>
       </c>
     </row>
@@ -917,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G12" s="15">
@@ -925,18 +928,18 @@
         <v>16.555555555555557</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1655.5555555555557</v>
       </c>
       <c r="I12" s="15">
         <v>20</v>
       </c>
       <c r="J12" s="16">
-        <f>I12-G12</f>
+        <f t="shared" si="0"/>
         <v>3.4444444444444429</v>
       </c>
       <c r="K12" s="16">
-        <f>J12*F12</f>
+        <f t="shared" si="1"/>
         <v>344.44444444444429</v>
       </c>
     </row>
@@ -955,9 +958,13 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
+    <row r="16" spans="1:11">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>